<commit_message>
heredity joint probability - child gene inheritance needs work
</commit_message>
<xml_diff>
--- a/project2/heredity/Heredity.xlsx
+++ b/project2/heredity/Heredity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/756f113a155ef17e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmfxy\gh\cs50ai\project2\heredity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="297" documentId="8_{4EC49F51-5A34-447C-A97C-3565F7EDB7B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1F7C8515-2584-4903-A846-0D81C96D5715}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BFFAB1-5D55-4212-9545-7944A8613D6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="1740" windowWidth="23220" windowHeight="13005" xr2:uid="{27E3B240-F815-4706-A81D-3A6EC469B2CF}"/>
+    <workbookView xWindow="2310" yWindow="1200" windowWidth="23220" windowHeight="13005" xr2:uid="{27E3B240-F815-4706-A81D-3A6EC469B2CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,13 +331,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBB296E-82F2-4E6F-8C0F-A71E6A5990DC}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,15 +736,15 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1033,13 +1033,13 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+      <c r="A42" s="5">
         <v>1</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="5">
         <v>0.5</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E42" t="s">
@@ -1072,10 +1072,10 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N47" s="6" t="s">
+      <c r="N47" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O47" s="6"/>
+      <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">

</xml_diff>